<commit_message>
Add a test file!
</commit_message>
<xml_diff>
--- a/Session10_Ta/minimum fluidization velocity_initialData (1).xlsx
+++ b/Session10_Ta/minimum fluidization velocity_initialData (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina\Documents\GitHub\CCRE_Fall_2023\Session10_Ta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6CFBA6-396F-4BBF-9569-6B342064B3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B73ABF-38E9-44CD-A994-A1FAC2481C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{B436F009-C256-45AF-8A86-3FC16F5F08B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>[-]</t>
   </si>
@@ -116,27 +116,9 @@
     <t>species</t>
   </si>
   <si>
-    <t>n-butane</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
     <t>H2O</t>
   </si>
   <si>
-    <t>N2</t>
-  </si>
-  <si>
     <t>mw</t>
   </si>
   <si>
@@ -204,6 +186,27 @@
   </si>
   <si>
     <t>vt/vmf</t>
+  </si>
+  <si>
+    <t>MeOH</t>
+  </si>
+  <si>
+    <t>DME</t>
+  </si>
+  <si>
+    <t>Ar</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>mole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vt </t>
+  </si>
+  <si>
+    <t>deltaP</t>
   </si>
 </sst>
 </file>
@@ -332,9 +335,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -372,7 +375,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -478,7 +481,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -620,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC43C87F-6A1A-44E3-803B-77CA0E49823B}">
-  <dimension ref="A3:P28"/>
+  <dimension ref="A3:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,34 +658,27 @@
         <v>25</v>
       </c>
       <c r="J3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="M3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>32</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4">
-        <f xml:space="preserve"> 27318</f>
-        <v>27318</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>9</v>
@@ -693,43 +689,40 @@
       </c>
       <c r="F4" s="4">
         <f xml:space="preserve"> B4/B5</f>
-        <v>22.765000000000001</v>
+        <v>7.874015748031497E-5</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J4" s="11">
-        <v>3.8461538461538498E-2</v>
+        <f xml:space="preserve"> J9/J10/$N$11</f>
+        <v>0.75172121597288433</v>
       </c>
       <c r="K4" s="11">
-        <v>0.20192307692307701</v>
-      </c>
-      <c r="L4" s="12">
+        <f t="shared" ref="K4:M4" si="0" xml:space="preserve"> K9/K10/$N$11</f>
         <v>0</v>
       </c>
-      <c r="M4" s="12">
+      <c r="L4" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N4" s="12">
-        <v>0</v>
-      </c>
-      <c r="O4" s="12">
-        <v>0</v>
-      </c>
-      <c r="P4" s="12">
-        <v>0.75961538461538503</v>
-      </c>
+      <c r="M4" s="11">
+        <f t="shared" si="0"/>
+        <v>0.24827878402711578</v>
+      </c>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4">
-        <f>1200</f>
-        <v>1200</v>
+        <v>1270</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -740,43 +733,36 @@
       </c>
       <c r="F5" s="7">
         <f xml:space="preserve"> 0.25 * PI()* B7^2</f>
-        <v>19.634954084936208</v>
+        <v>1.6619025137490004E-3</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J5" s="12">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="K5" s="12">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="L5" s="12">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="M5" s="12">
-        <v>28</v>
-      </c>
-      <c r="N5" s="12">
-        <v>44</v>
-      </c>
-      <c r="O5" s="12">
-        <v>18</v>
-      </c>
-      <c r="P5" s="12">
-        <v>28</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <f>0.42</f>
-        <v>0.42</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -787,64 +773,55 @@
       </c>
       <c r="F6" s="7">
         <f xml:space="preserve"> F4/(F5*(1-B6))</f>
-        <v>1.9989860852342052</v>
+        <v>7.9629459629403238E-2</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J6" s="11">
         <f>J5*J4</f>
-        <v>2.2307692307692331</v>
+        <v>24.055078911132298</v>
       </c>
       <c r="K6" s="11">
-        <f t="shared" ref="K6:P6" si="0">K5*K4</f>
-        <v>6.4615384615384643</v>
-      </c>
-      <c r="L6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K6:M6" si="1">K5*K4</f>
         <v>0</v>
       </c>
-      <c r="M6" s="12">
-        <f t="shared" si="0"/>
+      <c r="L6" s="11">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N6" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="12">
-        <f t="shared" si="0"/>
-        <v>21.269230769230781</v>
-      </c>
+      <c r="M6" s="11">
+        <f t="shared" si="1"/>
+        <v>9.9311513610846305</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4">
-        <f>5</f>
-        <v>5</v>
+        <f xml:space="preserve"> 0.046</f>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F7" s="4">
         <f xml:space="preserve"> SUM(J6:P6)</f>
-        <v>29.961538461538478</v>
+        <v>33.986230272216929</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -864,7 +841,7 @@
       </c>
       <c r="F8" s="4">
         <f xml:space="preserve"> B11*F7*0.001/(8.314*B12)</f>
-        <v>0.51930525915886272</v>
+        <v>0.7381261993384407</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>1</v>
@@ -875,22 +852,37 @@
         <v>18</v>
       </c>
       <c r="B9" s="4">
-        <f>0.000125</f>
-        <v>1.25E-4</v>
+        <f>0.000108</f>
+        <v>1.08E-4</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F9">
         <f xml:space="preserve"> PI()*B9^3/6</f>
-        <v>1.0226538585904275E-12</v>
+        <v>6.5958366080648421E-13</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9">
+        <v>0.7097</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0.29299999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -898,8 +890,8 @@
         <v>20</v>
       </c>
       <c r="B10" s="1">
-        <f>0.0000328</f>
-        <v>3.2799999999999998E-5</v>
+        <f>0.0000295</f>
+        <v>2.9499999999999999E-5</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>21</v>
@@ -908,6 +900,21 @@
       <c r="E10" s="1"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="12">
+        <v>32</v>
+      </c>
+      <c r="K10" s="12">
+        <v>46</v>
+      </c>
+      <c r="L10" s="12">
+        <v>18</v>
+      </c>
+      <c r="M10" s="12">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -923,14 +930,37 @@
       <c r="E11" s="1"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11">
+        <f>J9/J10</f>
+        <v>2.2178125E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:M11" si="2">K9/K10</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>7.3249999999999999E-3</v>
+      </c>
+      <c r="N11">
+        <f xml:space="preserve"> SUM(J11:M11)</f>
+        <v>2.9503124999999998E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="7">
-        <f xml:space="preserve"> 430 + 273.15</f>
-        <v>703.15</v>
+        <f xml:space="preserve"> 288 + 273.15</f>
+        <v>561.15</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>3</v>
@@ -951,23 +981,27 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4">
         <f xml:space="preserve"> 7/4*(1-B6)/B6^3*F8/B9</f>
-        <v>56915.542387025787</v>
+        <v>107126.47382287042</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="J14" s="15"/>
+      <c r="N14">
+        <f xml:space="preserve"> N11/(F5*F6)</f>
+        <v>222.94036406249995</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1">
         <f xml:space="preserve"> 150*(1-B6)^2/B6^3*B10/B9^2</f>
-        <v>1429727.2432782643</v>
+        <v>2021783.3974702349</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -975,11 +1009,11 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B16" s="4">
         <f xml:space="preserve"> -B4*B8/(F5*F6)</f>
-        <v>-6827.760000000002</v>
+        <v>-7412.9264999999996</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
@@ -991,71 +1025,72 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1">
         <f xml:space="preserve"> (-B15+SQRT(B15^2-4*B14*B16))/(2*B14)</f>
-        <v>4.7746606959990058E-3</v>
+        <v>3.6658164871501198E-3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F18" s="16">
         <f xml:space="preserve"> F8*B9*B20/B10</f>
-        <v>0.56016237595906682</v>
+        <v>5.9436650978092823E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1">
         <f>B18*1000</f>
-        <v>4.7746606959990059</v>
+        <v>3.6658164871501198</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F19" s="16">
         <f>24/F18</f>
-        <v>42.844719727755816</v>
+        <v>403.79125682646429</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B20" s="7">
-        <v>0.28304471187089181</v>
+        <f>B18*6</f>
+        <v>2.199489892290072E-2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F20" s="16">
         <f xml:space="preserve"> 24/F18*(1+0.15*F18^0.687)</f>
-        <v>47.160707831463682</v>
+        <v>412.50136392889789</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1">
         <f xml:space="preserve"> F9*(B5-F8)*B8-0.5*F8*B20^2*F20*PI()*B9^2*0.25</f>
-        <v>-5.6012974923230415E-12</v>
+        <v>7.538084122197236E-9</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1063,11 +1098,11 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B23" s="7">
         <f xml:space="preserve"> B20/B18</f>
-        <v>59.280591835158695</v>
+        <v>6</v>
       </c>
       <c r="C23" s="4"/>
       <c r="G23" s="4"/>
@@ -1078,28 +1113,36 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B25" s="7">
         <f xml:space="preserve"> 0.652*(F5*10000*(0.25*100-B18*100))^0.4</f>
-        <v>307.10415293121059</v>
+        <v>7.2293572505466148</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="1">
+        <f xml:space="preserve"> B9^2*B8*(1270-F8)/18/B10</f>
+        <v>0.27351001424833726</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <f xml:space="preserve"> B25/100</f>
-        <v>3.0710415293121058</v>
+        <v>7.2293572505466142E-2</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="7">
+        <f>G25/B18</f>
+        <v>74.610940074899787</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -1113,7 +1156,21 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
     </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="16">
+        <f xml:space="preserve"> F6*(150*(1-B6)^2/B6^3*B10*6*B18/B9^2)+(1.75*(1-B6)/B6^3*F8*(6*B18)^2/B9)</f>
+        <v>3592.8613589265974</v>
+      </c>
+      <c r="J30" s="16">
+        <f>6*B18</f>
+        <v>2.199489892290072E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>